<commit_message>
files OK, before Tallinn
</commit_message>
<xml_diff>
--- a/Account_starts_by_DD_and_profit/dd_trigger_optimization_results.xlsx
+++ b/Account_starts_by_DD_and_profit/dd_trigger_optimization_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vova deduskin lap\PycharmProjects\1500_count\Account_starts_by_DD_and_profit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B543341-CA7A-4DDB-8C24-A6C3D072EBB7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7261AA9D-F255-43AD-B90D-ED36492F42C7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,18 +76,12 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -117,14 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,19 +486,19 @@
         <v>500</v>
       </c>
       <c r="G2" s="2">
-        <v>3539414</v>
+        <v>187932</v>
       </c>
       <c r="H2">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="I2">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="J2">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>-214757</v>
+        <v>-14056</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -520,22 +512,22 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="G3" s="2">
-        <v>3531956</v>
+        <v>143067</v>
       </c>
       <c r="H3">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="I3">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="J3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>-212344</v>
+        <v>-9613</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -552,19 +544,19 @@
         <v>700</v>
       </c>
       <c r="G4" s="2">
-        <v>3529662</v>
+        <v>101427</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="I4">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="J4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>-219583</v>
+        <v>-6268</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -578,22 +570,22 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="G5" s="2">
-        <v>3525924</v>
+        <v>81792</v>
       </c>
       <c r="H5">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>-212344</v>
+        <v>-5195</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -607,22 +599,22 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="G6" s="2">
-        <v>3525740</v>
+        <v>53612</v>
       </c>
       <c r="H6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="J6">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>-209931</v>
+        <v>-3220</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -636,22 +628,22 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="G7" s="2">
-        <v>3503654</v>
+        <v>53295</v>
       </c>
       <c r="H7">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>-219583</v>
+        <v>-2994</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -665,22 +657,22 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="G8" s="2">
-        <v>3496602</v>
+        <v>32228</v>
       </c>
       <c r="H8">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>89</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K8">
-        <v>-214757</v>
+        <v>-2147</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -694,22 +686,22 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>900</v>
+        <v>2100</v>
       </c>
       <c r="G9" s="2">
-        <v>3421488</v>
+        <v>22240</v>
       </c>
       <c r="H9">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K9">
-        <v>-217170</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -723,22 +715,22 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1000</v>
+        <v>2900</v>
       </c>
       <c r="G10" s="2">
-        <v>3296872</v>
+        <v>22240</v>
       </c>
       <c r="H10">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K10">
-        <v>-227320</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -752,22 +744,22 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1100</v>
+        <v>2800</v>
       </c>
       <c r="G11" s="2">
-        <v>3128210</v>
+        <v>22240</v>
       </c>
       <c r="H11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>-183672</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -781,22 +773,22 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1200</v>
+        <v>2700</v>
       </c>
       <c r="G12" s="2">
-        <v>2903985</v>
+        <v>22240</v>
       </c>
       <c r="H12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>-176890</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -810,22 +802,22 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1300</v>
+        <v>2600</v>
       </c>
       <c r="G13" s="2">
-        <v>2853439</v>
+        <v>22240</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>-180614</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -839,22 +831,22 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>2500</v>
       </c>
       <c r="G14" s="2">
-        <v>2543465</v>
+        <v>22240</v>
       </c>
       <c r="H14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="K14">
-        <v>-144780</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -868,22 +860,22 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1400</v>
+        <v>2400</v>
       </c>
       <c r="G15" s="2">
-        <v>2373964</v>
+        <v>22240</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>-157466</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -897,22 +889,22 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1500</v>
+        <v>2300</v>
       </c>
       <c r="G16" s="2">
-        <v>2050965</v>
+        <v>22240</v>
       </c>
       <c r="H16">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
-        <v>-137325</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -926,22 +918,22 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1600</v>
+        <v>2200</v>
       </c>
       <c r="G17" s="2">
-        <v>1754100</v>
+        <v>22240</v>
       </c>
       <c r="H17">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>66</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>0</v>
       </c>
       <c r="K17">
-        <v>-119015</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -955,22 +947,22 @@
         <v>0</v>
       </c>
       <c r="E18">
-        <v>1700</v>
+        <v>1800</v>
       </c>
       <c r="G18" s="2">
-        <v>1577143</v>
+        <v>22240</v>
       </c>
       <c r="H18">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="I18">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>-106198</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -984,22 +976,22 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="G19" s="2">
-        <v>1274852</v>
+        <v>22240</v>
       </c>
       <c r="H19">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="I19">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>-86057</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1016,19 +1008,19 @@
         <v>1900</v>
       </c>
       <c r="G20" s="2">
-        <v>948674</v>
+        <v>22240</v>
       </c>
       <c r="H20">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="I20">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
-        <v>-63308</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1042,22 +1034,22 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>2000</v>
+        <v>1700</v>
       </c>
       <c r="G21" s="2">
-        <v>795284</v>
+        <v>22240</v>
       </c>
       <c r="H21">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="I21">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>-52136</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1071,51 +1063,51 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>2100</v>
+        <v>1600</v>
       </c>
       <c r="G22" s="2">
-        <v>598905</v>
+        <v>22240</v>
       </c>
       <c r="H22">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>-39102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B23" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="3">
-        <v>2200</v>
-      </c>
-      <c r="G23" s="4">
-        <v>469227</v>
-      </c>
-      <c r="H23" s="3">
-        <v>15</v>
-      </c>
-      <c r="I23" s="3">
-        <v>15</v>
-      </c>
-      <c r="J23" s="3">
-        <v>0</v>
-      </c>
-      <c r="K23" s="3">
-        <v>-27930</v>
+        <v>-1136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="b">
+        <v>0</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1500</v>
+      </c>
+      <c r="G23" s="2">
+        <v>22240</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>-1136</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1129,22 +1121,22 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>2300</v>
+        <v>1400</v>
       </c>
       <c r="G24" s="2">
-        <v>381243</v>
+        <v>22240</v>
       </c>
       <c r="H24">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
       </c>
       <c r="K24">
-        <v>-19132</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1158,22 +1150,22 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>2400</v>
+        <v>1300</v>
       </c>
       <c r="G25" s="2">
-        <v>320896</v>
+        <v>22240</v>
       </c>
       <c r="H25">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>-16891</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1187,22 +1179,22 @@
         <v>0</v>
       </c>
       <c r="E26">
-        <v>2500</v>
+        <v>1200</v>
       </c>
       <c r="G26" s="2">
-        <v>260458</v>
+        <v>22240</v>
       </c>
       <c r="H26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
-        <v>-14478</v>
+        <v>-1136</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1216,138 +1208,22 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>2600</v>
+        <v>3000</v>
       </c>
       <c r="G27" s="2">
-        <v>217652</v>
+        <v>22240</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
-        <v>-12065</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="b">
-        <v>0</v>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
-      </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>2700</v>
-      </c>
-      <c r="G28" s="2">
-        <v>217652</v>
-      </c>
-      <c r="H28">
-        <v>5</v>
-      </c>
-      <c r="I28">
-        <v>5</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>-12065</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="b">
-        <v>0</v>
-      </c>
-      <c r="B29" t="b">
-        <v>1</v>
-      </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>2800</v>
-      </c>
-      <c r="G29" s="2">
-        <v>131710</v>
-      </c>
-      <c r="H29">
-        <v>3</v>
-      </c>
-      <c r="I29">
-        <v>3</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>-7239</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="b">
-        <v>0</v>
-      </c>
-      <c r="B30" t="b">
-        <v>1</v>
-      </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>2900</v>
-      </c>
-      <c r="G30" s="2">
-        <v>131710</v>
-      </c>
-      <c r="H30">
-        <v>3</v>
-      </c>
-      <c r="I30">
-        <v>3</v>
-      </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>-7239</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="b">
-        <v>0</v>
-      </c>
-      <c r="B31" t="b">
-        <v>1</v>
-      </c>
-      <c r="C31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>3000</v>
-      </c>
-      <c r="G31" s="2">
-        <v>88565</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>-4826</v>
+        <v>-1136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>